<commit_message>
Some changes and some deletions nothing special
</commit_message>
<xml_diff>
--- a/Testflightdata/20200305_V3.xlsx
+++ b/Testflightdata/20200305_V3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Documents\TU Delft\BSc-3\AE3212-II Simulation, Verification &amp; Validation\Aerodynamics\31\B31\Testflightdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/088ac5db3e9756e7/Documents/MATLAB/31/B31/Testflightdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D9673C-669A-48EE-84EB-126651A6B02F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{87D9673C-669A-48EE-84EB-126651A6B02F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{25E8A786-7441-444D-8C99-FB49118896D8}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-5600" windowWidth="38620" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="1900" windowWidth="30470" windowHeight="17170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imperial Units" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -507,8 +507,8 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -969,24 +969,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5.8386682072143845E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.3301208723085525E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.009585658731935E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3887680307737106E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.914788131248011E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3697841964277998E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1440,22 +1422,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1466,24 +1448,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5.8386682072143845E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.3301208723085525E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.009585658731935E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3887680307737106E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.914788131248011E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3697841964277998E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1890,22 +1854,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9514,51 +9478,33 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="28">
-          <cell r="F28">
-            <v>1.8</v>
-          </cell>
-          <cell r="Q28">
-            <v>5.8386682072143845E-3</v>
+          <cell r="F28" t="e">
+            <v>#REF!</v>
           </cell>
         </row>
         <row r="29">
-          <cell r="F29">
-            <v>2.5</v>
-          </cell>
-          <cell r="Q29">
-            <v>7.3301208723085525E-3</v>
+          <cell r="F29" t="e">
+            <v>#REF!</v>
           </cell>
         </row>
         <row r="30">
-          <cell r="F30">
-            <v>3.9</v>
-          </cell>
-          <cell r="Q30">
-            <v>1.009585658731935E-2</v>
+          <cell r="F30" t="e">
+            <v>#REF!</v>
           </cell>
         </row>
         <row r="31">
-          <cell r="F31">
-            <v>5.7</v>
-          </cell>
-          <cell r="Q31">
-            <v>1.3887680307737106E-2</v>
+          <cell r="F31" t="e">
+            <v>#REF!</v>
           </cell>
         </row>
         <row r="32">
-          <cell r="F32">
-            <v>8.1999999999999993</v>
-          </cell>
-          <cell r="Q32">
-            <v>1.914788131248011E-2</v>
+          <cell r="F32" t="e">
+            <v>#REF!</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="F33">
-            <v>10.3</v>
-          </cell>
-          <cell r="Q33">
-            <v>2.3697841964277998E-2</v>
+          <cell r="F33" t="e">
+            <v>#REF!</v>
           </cell>
         </row>
       </sheetData>
@@ -9894,21 +9840,21 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="8.15625" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="7.15625" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
     <col min="5" max="13" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -9920,7 +9866,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9932,13 +9878,13 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -9946,7 +9892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -9957,7 +9903,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -9968,7 +9914,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -9979,7 +9925,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -9990,7 +9936,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -10001,7 +9947,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -10012,7 +9958,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -10023,7 +9969,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -10034,7 +9980,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -10045,7 +9991,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -10053,12 +9999,12 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -10066,7 +10012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -10098,7 +10044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
@@ -10127,7 +10073,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
@@ -10160,7 +10106,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -10193,7 +10139,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3</v>
       </c>
@@ -10226,7 +10172,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>4</v>
       </c>
@@ -10259,7 +10205,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>5</v>
       </c>
@@ -10292,7 +10238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>6</v>
       </c>
@@ -10325,7 +10271,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>7</v>
       </c>
@@ -10339,23 +10285,23 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="E39" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -10387,7 +10333,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B42" s="5" t="s">
         <v>58</v>
       </c>
@@ -10416,7 +10362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
@@ -10430,7 +10376,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
@@ -10444,7 +10390,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>3</v>
       </c>
@@ -10458,7 +10404,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>4</v>
       </c>
@@ -10472,7 +10418,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>5</v>
       </c>
@@ -10486,7 +10432,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>6</v>
       </c>
@@ -10500,7 +10446,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>7</v>
       </c>
@@ -10514,17 +10460,17 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C51" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -10532,7 +10478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -10573,7 +10519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B57" s="5" t="s">
         <v>58</v>
       </c>
@@ -10611,7 +10557,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
@@ -10652,7 +10598,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
@@ -10693,7 +10639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>3</v>
       </c>
@@ -10734,7 +10680,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>4</v>
       </c>
@@ -10775,7 +10721,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>5</v>
       </c>
@@ -10816,7 +10762,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>6</v>
       </c>
@@ -10857,7 +10803,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>7</v>
       </c>
@@ -10898,17 +10844,17 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C66" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -10916,7 +10862,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>57</v>
       </c>
@@ -10930,7 +10876,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -10971,7 +10917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B74" s="5" t="s">
         <v>58</v>
       </c>
@@ -11009,7 +10955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
@@ -11050,7 +10996,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2</v>
       </c>
@@ -11091,17 +11037,17 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C77" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D81" t="s">
         <v>36</v>
       </c>
@@ -11112,7 +11058,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D82" t="s">
         <v>58</v>
       </c>
@@ -11123,7 +11069,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -11143,7 +11089,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>40</v>
       </c>
@@ -11261,20 +11207,20 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U46" sqref="U46"/>
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1015625" customWidth="1"/>
-    <col min="12" max="12" width="10.68359375" customWidth="1"/>
-    <col min="15" max="15" width="15.62890625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.68359375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.08984375" customWidth="1"/>
+    <col min="12" max="12" width="10.6328125" customWidth="1"/>
+    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -11295,7 +11241,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="G2" t="s">
         <v>100</v>
       </c>
@@ -11320,7 +11266,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -11340,7 +11286,7 @@
         <v>2.0569000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -11358,7 +11304,7 @@
         <v>1859.7287170000002</v>
       </c>
       <c r="Q4" s="18">
-        <f t="shared" ref="Q3:Q33" si="0">P4*9.80665</f>
+        <f t="shared" ref="Q4:Q33" si="0">P4*9.80665</f>
         <v>18237.70862256805</v>
       </c>
       <c r="S4" s="19" t="s">
@@ -11368,7 +11314,7 @@
         <v>15.911</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="O5" s="21"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="18"/>
@@ -11380,7 +11326,7 @@
         <v>8.4386640333333336</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -11388,7 +11334,7 @@
         <v>99</v>
       </c>
       <c r="P6" s="16">
-        <f>D8</f>
+        <f t="shared" ref="P6:P14" si="1">D8</f>
         <v>80</v>
       </c>
       <c r="Q6" s="18">
@@ -11405,13 +11351,13 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="O7" s="21"/>
       <c r="P7" s="16">
-        <f>D9</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="Q7" s="18">
@@ -11428,7 +11374,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -11442,7 +11388,7 @@
       </c>
       <c r="O8" s="21"/>
       <c r="P8" s="16">
-        <f>D10</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="Q8" s="18">
@@ -11450,7 +11396,7 @@
         <v>588.399</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -11464,7 +11410,7 @@
       </c>
       <c r="O9" s="21"/>
       <c r="P9" s="16">
-        <f>D11</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="Q9" s="18">
@@ -11472,7 +11418,7 @@
         <v>735.49874999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -11486,7 +11432,7 @@
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="16">
-        <f>D12</f>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="Q10" s="18">
@@ -11494,7 +11440,7 @@
         <v>813.9519499999999</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -11508,7 +11454,7 @@
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="16">
-        <f>D13</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="Q11" s="18">
@@ -11516,7 +11462,7 @@
         <v>647.23889999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -11530,7 +11476,7 @@
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="16">
-        <f>D14</f>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="Q12" s="18">
@@ -11538,7 +11484,7 @@
         <v>872.79184999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -11552,7 +11498,7 @@
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="16">
-        <f>D15</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="Q13" s="18">
@@ -11560,7 +11506,7 @@
         <v>833.56524999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -11574,7 +11520,7 @@
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="16">
-        <f>D16</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="Q14" s="18">
@@ -11582,7 +11528,7 @@
         <v>882.59849999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -11598,7 +11544,7 @@
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -11622,28 +11568,28 @@
         <v>66164.514226430532</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O17" s="21"/>
       <c r="P17" s="16"/>
       <c r="Q17" s="18"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D18" s="15"/>
       <c r="O18" s="21"/>
       <c r="P18" s="16"/>
       <c r="Q18" s="18"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O19" s="21"/>
       <c r="P19" s="16"/>
       <c r="Q19" s="18"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O20" s="21"/>
       <c r="P20" s="16"/>
       <c r="Q20" s="18"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>78</v>
       </c>
@@ -11651,12 +11597,12 @@
       <c r="P21" s="16"/>
       <c r="Q21" s="18"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O22" s="21"/>
       <c r="P22" s="16"/>
       <c r="Q22" s="18"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -11667,12 +11613,12 @@
       <c r="P23" s="16"/>
       <c r="Q23" s="18"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O24" s="21"/>
       <c r="P24" s="16"/>
       <c r="Q24" s="18"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -11710,7 +11656,7 @@
       <c r="P25" s="16"/>
       <c r="Q25" s="18"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>58</v>
       </c>
@@ -11742,7 +11688,7 @@
       <c r="P26" s="16"/>
       <c r="Q26" s="18"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O27" s="21"/>
       <c r="P27" s="16"/>
       <c r="Q27" s="18"/>
@@ -11756,7 +11702,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
@@ -11816,7 +11762,7 @@
         <v>0.21679976422288083</v>
       </c>
       <c r="S28" s="27">
-        <f>$T$6+R28^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" ref="S28:S33" si="2">$T$6+R28^2/(PI()*$T$5*$T$7)</f>
         <v>4.2216175016557923E-2</v>
       </c>
       <c r="T28" s="28">
@@ -11824,7 +11770,7 @@
         <v>4.7002137767096719E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -11833,7 +11779,7 @@
         <v>0.72152777777777777</v>
       </c>
       <c r="C29" s="8">
-        <f t="shared" ref="C29:C33" si="1">B29-$B$28</f>
+        <f t="shared" ref="C29:C33" si="3">B29-$B$28</f>
         <v>6.944444444444442E-2</v>
       </c>
       <c r="D29" s="9">
@@ -11865,14 +11811,14 @@
         <v>8.5</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" ref="K29:K33" si="2">E29/SQRT(1.4*287*(J29+273.15))</f>
+        <f t="shared" ref="K29:K33" si="4">E29/SQRT(1.4*287*(J29+273.15))</f>
         <v>0.3379640735189966</v>
       </c>
       <c r="O29" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P29" s="18">
-        <f t="shared" ref="P29:P33" si="3">$P$16-I29</f>
+        <f t="shared" ref="P29:P33" si="5">$P$16-I29</f>
         <v>6595.40293647</v>
       </c>
       <c r="Q29" s="18">
@@ -11880,19 +11826,19 @@
         <v>64678.808206933521</v>
       </c>
       <c r="R29" s="27">
-        <f t="shared" ref="R29:R33" si="4">2*Q29/(1.225*E29^2*$T$2)</f>
+        <f t="shared" ref="R29:R33" si="6">2*Q29/(1.225*E29^2*$T$2)</f>
         <v>0.27231646512747643</v>
       </c>
       <c r="S29" s="27">
-        <f>$T$6+R29^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" si="2"/>
         <v>4.3496505739740031E-2</v>
       </c>
       <c r="T29" s="28">
-        <f t="shared" ref="T29:T33" si="5">R29^2</f>
+        <f t="shared" ref="T29:T33" si="7">R29^2</f>
         <v>7.4156257179524079E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3</v>
       </c>
@@ -11901,7 +11847,7 @@
         <v>0.80555555555555547</v>
       </c>
       <c r="C30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.15347222222222212</v>
       </c>
       <c r="D30" s="9">
@@ -11933,14 +11879,14 @@
         <v>6.8</v>
       </c>
       <c r="K30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.28837044891924335</v>
       </c>
       <c r="O30" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P30" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6582.7023501100002</v>
       </c>
       <c r="Q30" s="18">
@@ -11948,19 +11894,19 @@
         <v>64554.258001706228</v>
       </c>
       <c r="R30" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.37558274748152998</v>
       </c>
       <c r="S30" s="27">
-        <f>$T$6+R30^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" si="2"/>
         <v>4.6651164861071029E-2</v>
       </c>
       <c r="T30" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.14106240020577471</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>4</v>
       </c>
@@ -11969,7 +11915,7 @@
         <v>0.89722222222222225</v>
       </c>
       <c r="C31" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.24513888888888891</v>
       </c>
       <c r="D31" s="9">
@@ -12001,14 +11947,14 @@
         <v>5.2</v>
       </c>
       <c r="K31" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.24612600925785433</v>
       </c>
       <c r="O31" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P31" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6565.9194324199998</v>
       </c>
       <c r="Q31" s="18">
@@ -12016,19 +11962,19 @@
         <v>64389.673801941586</v>
       </c>
       <c r="R31" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.51721689068414878</v>
       </c>
       <c r="S31" s="27">
-        <f>$T$6+R31^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" si="2"/>
         <v>5.2613390514462628E-2</v>
       </c>
       <c r="T31" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.26751331200897871</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>5</v>
       </c>
@@ -12037,7 +11983,7 @@
         <v>0.95694444444444438</v>
       </c>
       <c r="C32" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30486111111111103</v>
       </c>
       <c r="D32" s="9">
@@ -12069,14 +12015,14 @@
         <v>4</v>
       </c>
       <c r="K32" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.209659529607583</v>
       </c>
       <c r="O32" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P32" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6557.3011773899998</v>
       </c>
       <c r="Q32" s="18">
@@ -12084,19 +12030,19 @@
         <v>64305.157591251635</v>
       </c>
       <c r="R32" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.71493149515459753</v>
       </c>
       <c r="S32" s="27">
-        <f>$T$6+R32^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" si="2"/>
         <v>6.4099903457022128E-2</v>
       </c>
       <c r="T32" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.51112704276398835</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>6</v>
       </c>
@@ -12104,7 +12050,7 @@
         <v>2.0187499999999998</v>
       </c>
       <c r="C33" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3666666666666665</v>
       </c>
       <c r="D33" s="9">
@@ -12136,14 +12082,14 @@
         <v>3.8</v>
       </c>
       <c r="K33" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.18814482878273514</v>
       </c>
       <c r="O33" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P33" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6546.8685528799997</v>
       </c>
       <c r="Q33" s="18">
@@ -12151,19 +12097,19 @@
         <v>64202.848494100646</v>
       </c>
       <c r="R33" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.88701522655592502</v>
       </c>
       <c r="S33" s="27">
-        <f>$T$6+R33^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" si="2"/>
         <v>7.7097837419158349E-2</v>
       </c>
       <c r="T33" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.78679601214205896</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>7</v>
       </c>
@@ -12172,7 +12118,7 @@
       <c r="P34" s="16"/>
       <c r="Q34" s="16"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>43</v>
       </c>
@@ -12180,12 +12126,12 @@
       <c r="P35" s="16"/>
       <c r="Q35" s="16"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O36" s="21"/>
       <c r="P36" s="16"/>
       <c r="Q36" s="16"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -12193,12 +12139,12 @@
       <c r="P37" s="16"/>
       <c r="Q37" s="16"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O38" s="21"/>
       <c r="P38" s="16"/>
       <c r="Q38" s="16"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -12206,12 +12152,12 @@
       <c r="P39" s="16"/>
       <c r="Q39" s="16"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O40" s="21"/>
       <c r="P40" s="16"/>
       <c r="Q40" s="16"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -12246,7 +12192,7 @@
       <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>58</v>
       </c>
@@ -12278,12 +12224,12 @@
       <c r="P42" s="16"/>
       <c r="Q42" s="16"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O43" s="21"/>
       <c r="P43" s="16"/>
       <c r="Q43" s="16"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
@@ -12327,7 +12273,7 @@
       <c r="P44" s="16"/>
       <c r="Q44" s="16"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
@@ -12336,7 +12282,7 @@
         <v>0</v>
       </c>
       <c r="C45" s="8">
-        <f t="shared" ref="C45:C49" si="6">B45-$B$28</f>
+        <f t="shared" ref="C45:C49" si="8">B45-$B$28</f>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D45" s="9">
@@ -12371,7 +12317,7 @@
       <c r="P45" s="16"/>
       <c r="Q45" s="16"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>3</v>
       </c>
@@ -12380,7 +12326,7 @@
         <v>0</v>
       </c>
       <c r="C46" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D46" s="9">
@@ -12415,7 +12361,7 @@
       <c r="P46" s="16"/>
       <c r="Q46" s="16"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>4</v>
       </c>
@@ -12424,7 +12370,7 @@
         <v>0</v>
       </c>
       <c r="C47" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D47" s="9">
@@ -12459,7 +12405,7 @@
       <c r="P47" s="16"/>
       <c r="Q47" s="16"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>5</v>
       </c>
@@ -12468,7 +12414,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D48" s="9">
@@ -12503,13 +12449,13 @@
       <c r="P48" s="16"/>
       <c r="Q48" s="16"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>6</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D49" s="9">
@@ -12544,7 +12490,7 @@
       <c r="P49" s="16"/>
       <c r="Q49" s="16"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>7</v>
       </c>
@@ -12553,12 +12499,12 @@
       <c r="P50" s="16"/>
       <c r="Q50" s="16"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O51" s="21"/>
       <c r="P51" s="16"/>
       <c r="Q51" s="16"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>28</v>
       </c>
@@ -12566,12 +12512,12 @@
       <c r="P52" s="16"/>
       <c r="Q52" s="16"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O53" s="21"/>
       <c r="P53" s="16"/>
       <c r="Q53" s="16"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -12582,12 +12528,12 @@
       <c r="P54" s="16"/>
       <c r="Q54" s="16"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O55" s="21"/>
       <c r="P55" s="16"/>
       <c r="Q55" s="16"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -12631,7 +12577,7 @@
       <c r="P56" s="16"/>
       <c r="Q56" s="16"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>58</v>
       </c>
@@ -12672,12 +12618,12 @@
       <c r="P57" s="16"/>
       <c r="Q57" s="16"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
       <c r="O58" s="21"/>
       <c r="P58" s="16"/>
       <c r="Q58" s="16"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
@@ -12741,7 +12687,7 @@
         <v>6504.2308701000002</v>
       </c>
       <c r="Q59" s="18">
-        <f t="shared" ref="Q59:Q65" si="7">P59*9.80665</f>
+        <f t="shared" ref="Q59:Q65" si="9">P59*9.80665</f>
         <v>63784.715662266164</v>
       </c>
       <c r="R59" s="29">
@@ -12749,7 +12695,7 @@
         <v>0.51235750020238557</v>
       </c>
       <c r="S59" s="29">
-        <f>$T$6+R59^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" ref="S59:S65" si="10">$T$6+R59^2/(PI()*$T$5*$T$7)</f>
         <v>5.2377491582914923E-2</v>
       </c>
       <c r="T59" s="30">
@@ -12757,7 +12703,7 @@
         <v>0.26251020801363756</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
@@ -12810,34 +12756,34 @@
         <v>2</v>
       </c>
       <c r="N60" s="9">
-        <f t="shared" ref="N60:N65" si="8">E60/SQRT(1.4*287*(J29+273.15))</f>
+        <f t="shared" ref="N60:N65" si="11">E60/SQRT(1.4*287*(J29+273.15))</f>
         <v>0.22785813101507013</v>
       </c>
       <c r="O60" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P60" s="18">
-        <f t="shared" ref="P60:P65" si="9">$P$16-L60</f>
+        <f t="shared" ref="P60:P65" si="12">$P$16-L60</f>
         <v>6494.2518379599996</v>
       </c>
       <c r="Q60" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>63686.85478673043</v>
       </c>
       <c r="R60" s="29">
-        <f t="shared" ref="R60:R64" si="10">2*Q60/(1.225*E60^2*$T$2)</f>
+        <f t="shared" ref="R60:R64" si="13">2*Q60/(1.225*E60^2*$T$2)</f>
         <v>0.58989362693827274</v>
       </c>
       <c r="S60" s="29">
-        <f>$T$6+R60^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" si="10"/>
         <v>5.6407176571454255E-2</v>
       </c>
       <c r="T60" s="30">
-        <f t="shared" ref="T60:T64" si="11">R60^2</f>
+        <f t="shared" ref="T60:T64" si="14">R60^2</f>
         <v>0.34797449110239009</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>3</v>
       </c>
@@ -12890,34 +12836,34 @@
         <v>1.5</v>
       </c>
       <c r="N61" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.21474395132284077</v>
       </c>
       <c r="O61" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P61" s="18">
+        <f t="shared" si="12"/>
+        <v>6489.2623218899998</v>
+      </c>
+      <c r="Q61" s="18">
         <f t="shared" si="9"/>
-        <v>6489.2623218899998</v>
-      </c>
-      <c r="Q61" s="18">
-        <f t="shared" si="7"/>
         <v>63637.924348962566</v>
       </c>
       <c r="R61" s="29">
+        <f t="shared" si="13"/>
+        <v>0.66766156198440596</v>
+      </c>
+      <c r="S61" s="29">
         <f t="shared" si="10"/>
-        <v>0.66766156198440596</v>
-      </c>
-      <c r="S61" s="29">
-        <f>$T$6+R61^2/(PI()*$T$5*$T$7)</f>
         <v>6.1018377690061076E-2</v>
       </c>
       <c r="T61" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.44577196135145675</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>4</v>
       </c>
@@ -12970,34 +12916,34 @@
         <v>0.8</v>
       </c>
       <c r="N62" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.19997738252200661</v>
       </c>
       <c r="O62" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P62" s="18">
+        <f t="shared" si="12"/>
+        <v>6478.3761050100002</v>
+      </c>
+      <c r="Q62" s="18">
         <f t="shared" si="9"/>
-        <v>6478.3761050100002</v>
-      </c>
-      <c r="Q62" s="18">
-        <f t="shared" si="7"/>
         <v>63531.167030196317</v>
       </c>
       <c r="R62" s="29">
+        <f t="shared" si="13"/>
+        <v>0.77303039075602054</v>
+      </c>
+      <c r="S62" s="29">
         <f t="shared" si="10"/>
-        <v>0.77303039075602054</v>
-      </c>
-      <c r="S62" s="29">
-        <f>$T$6+R62^2/(PI()*$T$5*$T$7)</f>
         <v>6.8176015633290898E-2</v>
       </c>
       <c r="T62" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.59757598503240583</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>5</v>
       </c>
@@ -13050,34 +12996,34 @@
         <v>3.2</v>
       </c>
       <c r="N63" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.26361602619776986</v>
       </c>
       <c r="O63" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P63" s="18">
+        <f t="shared" si="12"/>
+        <v>6467.4898881299996</v>
+      </c>
+      <c r="Q63" s="18">
         <f t="shared" si="9"/>
-        <v>6467.4898881299996</v>
-      </c>
-      <c r="Q63" s="18">
-        <f t="shared" si="7"/>
         <v>63424.40971143006</v>
       </c>
       <c r="R63" s="29">
+        <f t="shared" si="13"/>
+        <v>0.4460264899510662</v>
+      </c>
+      <c r="S63" s="29">
         <f t="shared" si="10"/>
-        <v>0.4460264899510662</v>
-      </c>
-      <c r="S63" s="29">
-        <f>$T$6+R63^2/(PI()*$T$5*$T$7)</f>
         <v>4.9380106058440343E-2</v>
       </c>
       <c r="T63" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.19893962973806856</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>6</v>
       </c>
@@ -13130,34 +13076,34 @@
         <v>4.2</v>
       </c>
       <c r="N64" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.28067507244637535</v>
       </c>
       <c r="O64" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P64" s="18">
+        <f t="shared" si="12"/>
+        <v>6458.8716330999996</v>
+      </c>
+      <c r="Q64" s="18">
         <f t="shared" si="9"/>
-        <v>6458.8716330999996</v>
-      </c>
-      <c r="Q64" s="18">
-        <f t="shared" si="7"/>
         <v>63339.893500740109</v>
       </c>
       <c r="R64" s="29">
+        <f t="shared" si="13"/>
+        <v>0.39321582917293663</v>
+      </c>
+      <c r="S64" s="29">
         <f t="shared" si="10"/>
-        <v>0.39321582917293663</v>
-      </c>
-      <c r="S64" s="29">
-        <f>$T$6+R64^2/(PI()*$T$5*$T$7)</f>
         <v>4.7290350831026291E-2</v>
       </c>
       <c r="T64" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.15461868831216008</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>7</v>
       </c>
@@ -13210,34 +13156,34 @@
         <v>6.8</v>
       </c>
       <c r="N65" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.29504355938219456</v>
       </c>
       <c r="O65" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P65" s="18">
+        <f t="shared" si="12"/>
+        <v>6442.9959001500001</v>
+      </c>
+      <c r="Q65" s="18">
         <f t="shared" si="9"/>
-        <v>6442.9959001500001</v>
-      </c>
-      <c r="Q65" s="18">
-        <f t="shared" si="7"/>
         <v>63184.205744205996</v>
       </c>
       <c r="R65" s="29">
-        <f t="shared" ref="R65" si="12">2*Q65/(1.225*E65^2*$T$2)</f>
+        <f t="shared" ref="R65" si="15">2*Q65/(1.225*E65^2*$T$2)</f>
         <v>0.35991319439458458</v>
       </c>
       <c r="S65" s="29">
-        <f>$T$6+R65^2/(PI()*$T$5*$T$7)</f>
+        <f t="shared" si="10"/>
         <v>4.6107760231027826E-2</v>
       </c>
       <c r="T65" s="30">
-        <f t="shared" ref="T65" si="13">R65^2</f>
+        <f t="shared" ref="T65" si="16">R65^2</f>
         <v>0.12953750749931403</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
       <c r="N66" s="9"/>
       <c r="O66" s="21"/>
       <c r="P66" s="16"/>
@@ -13246,7 +13192,7 @@
       <c r="S66" s="9"/>
       <c r="T66" s="9"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
       <c r="N67" s="9"/>
       <c r="O67" s="21"/>
       <c r="P67" s="16"/>
@@ -13255,7 +13201,7 @@
       <c r="S67" s="9"/>
       <c r="T67" s="9"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>33</v>
       </c>
@@ -13267,7 +13213,7 @@
       <c r="S68" s="9"/>
       <c r="T68" s="9"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
       <c r="N69" s="9"/>
       <c r="O69" s="21"/>
       <c r="P69" s="16"/>
@@ -13276,7 +13222,7 @@
       <c r="S69" s="9"/>
       <c r="T69" s="9"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -13291,7 +13237,7 @@
       <c r="S70" s="9"/>
       <c r="T70" s="9"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -13312,7 +13258,7 @@
       <c r="S71" s="9"/>
       <c r="T71" s="9"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
       <c r="N72" s="9"/>
       <c r="O72" s="21"/>
       <c r="P72" s="16"/>
@@ -13321,7 +13267,7 @@
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -13369,7 +13315,7 @@
       <c r="S73" s="9"/>
       <c r="T73" s="9"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>58</v>
       </c>
@@ -13414,7 +13360,7 @@
       <c r="S74" s="9"/>
       <c r="T74" s="9"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
@@ -13467,22 +13413,22 @@
         <v>4.2</v>
       </c>
       <c r="N75" s="9">
-        <f t="shared" ref="N75:N76" si="14">E75/SQRT(1.4*287*(J44+273.15))</f>
+        <f t="shared" ref="N75:N76" si="17">E75/SQRT(1.4*287*(J44+273.15))</f>
         <v>0.24690487337773126</v>
       </c>
       <c r="O75" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P75" s="18">
-        <f t="shared" ref="P75" si="15">$P$16-L75</f>
+        <f t="shared" ref="P75" si="18">$P$16-L75</f>
         <v>6429.8417214199999</v>
       </c>
       <c r="Q75" s="18">
-        <f t="shared" ref="Q75:Q76" si="16">P75*9.80665</f>
+        <f t="shared" ref="Q75:Q76" si="19">P75*9.80665</f>
         <v>63055.207317363442</v>
       </c>
       <c r="R75" s="29">
-        <f t="shared" ref="R75:R76" si="17">2*Q75/(1.225*E75^2*$T$2)</f>
+        <f t="shared" ref="R75:R76" si="20">2*Q75/(1.225*E75^2*$T$2)</f>
         <v>0.51288872127463514</v>
       </c>
       <c r="S75" s="29">
@@ -13490,11 +13436,11 @@
         <v>5.2403171281094313E-2</v>
       </c>
       <c r="T75" s="30">
-        <f t="shared" ref="T75:T76" si="18">R75^2</f>
+        <f t="shared" ref="T75:T76" si="21">R75^2</f>
         <v>0.26305484041073035</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2</v>
       </c>
@@ -13547,22 +13493,22 @@
         <v>4.2</v>
       </c>
       <c r="N76" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.24535201253887759</v>
       </c>
       <c r="O76" s="21" t="s">
         <v>102</v>
       </c>
       <c r="P76" s="18">
-        <f t="shared" ref="P76" si="19">$P$16-L76</f>
+        <f t="shared" ref="P76" si="22">$P$16-L76</f>
         <v>6417.5947274299997</v>
       </c>
       <c r="Q76" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>62935.105333751402</v>
       </c>
       <c r="R76" s="29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.5184122185962482</v>
       </c>
       <c r="S76" s="29">
@@ -13570,16 +13516,16 @@
         <v>5.2671758909737437E-2</v>
       </c>
       <c r="T76" s="30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.26875122838988424</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D81" t="s">
         <v>36</v>
       </c>
@@ -13590,7 +13536,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D82" t="s">
         <v>58</v>
       </c>
@@ -13601,7 +13547,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -13628,7 +13574,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>40</v>
       </c>

</xml_diff>